<commit_message>
add active skill type
</commit_message>
<xml_diff>
--- a/skillbase.xlsx
+++ b/skillbase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-1860" yWindow="3705" windowWidth="18195" windowHeight="7545"/>
@@ -2279,7 +2279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="184">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2393,639 +2393,635 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>SKILL_NAME_1600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buffer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uncommon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_buffer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>soul.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>magic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_2400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_2400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal_heal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assist_heal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>soul.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>magic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>physic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uncommon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instant_kill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;eventtarget,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;eventtarget,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hppercent,0.7,particles/taken-gem.plist,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1401</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1401</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valuebase_heal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtarget,2000,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1601</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1601</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buffer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>physic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;enemy,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;enemy,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>soul.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>physic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtrigger,1000,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>battle_init</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>magic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtrigger,5000,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtrigger,5001,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>battle_init</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beDefender</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ally_except_me</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1203</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1203</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>counter_attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1602</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1602</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buffer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>magic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtarget,2001,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtarget,1001,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1603</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1603</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtarget,1002,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1605</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1605</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>soul.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;enemy,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,alive,1;enemy,alive,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal_attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal_attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profession_class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy,1,attack,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ally,-1,heal,1,particles/taken-gem.plist,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack,1,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_6000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_6000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_3001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_3001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_3002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_3002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy,1,Attack,4,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_3003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_3003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_6001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_6001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,1003,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,1000,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_6002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_6002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,5002,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_4001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_4001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ally,1,Heal,1,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_3004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_3004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_6003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_6003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,5003,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_3005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_3005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal_magic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy,2,Attack,1.5,particles/taken-gem.plist,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy,-1,Attack,0.9,particles/taken-gem.plist,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy,4000,particles/taken-gem.plist,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy,2000,particles/taken-gem.plist,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_3006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_3006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_6004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_6004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,5004,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self,1,0.5,particles/taken-gem.plist,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_3007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_3007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shoot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtarget,1004,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,3,boarder_left.png,particles/taken-gem.plist,particles/taken-gem.plist,line,Attack,0.9,0.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multi_attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1606</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1606</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_NAME_1607</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL_DESC_1607</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtarget,3000,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventtarget,1006,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy,4001,particles/taken-gem.plist,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy,1005,particles/taken-gem.plist,1,particles/taken-gem.plist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>action</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SKILL_NAME_1600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buffer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uncommon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add_buffer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>soul.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>magic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>heal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rare</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_2400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_2400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normal_heal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>assist_heal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>soul.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>defense</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>magic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>physic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uncommon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>instant_kill</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;eventtarget,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;eventtarget,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hppercent,0.7,particles/taken-gem.plist,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1401</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1401</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>heal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>valuebase_heal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtarget,2000,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1601</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1601</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buffer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>physic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;enemy,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;enemy,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>soul.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>physic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtrigger,1000,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>battle_init</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>defense</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>magic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtrigger,5000,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtrigger,5001,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>battle_init</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1202</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1202</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>beDefender</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ally_except_me</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>guard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1203</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1203</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>counter_attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1602</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1602</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buffer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>magic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rare</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtarget,2001,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtarget,1001,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1603</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1603</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtarget,1002,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1605</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1605</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>soul.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>common</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;enemy,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,alive,1;enemy,alive,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normal_attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normal_attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>profession_class</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemy,1,attack,1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ally,-1,heal,1,particles/taken-gem.plist,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attack,1,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_6000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_6000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_3001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_3001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_3002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_3002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemy,1,Attack,4,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_3003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_3003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_6001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_6001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,1003,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,1000,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_6002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_6002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,5002,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_4001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_4001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ally,1,Heal,1,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_3004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_3004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_6003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_6003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,5003,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_3005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_3005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normal_magic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemy,2,Attack,1.5,particles/taken-gem.plist,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemy,-1,Attack,0.9,particles/taken-gem.plist,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemy,4000,particles/taken-gem.plist,1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemy,2000,particles/taken-gem.plist,1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_3006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_3006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_6004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_6004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,5004,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>self,1,0.5,particles/taken-gem.plist,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_3007</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_3007</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shoot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtarget,1004,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5,3,boarder_left.png,particles/taken-gem.plist,particles/taken-gem.plist,line,Attack,0.9,0.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>multi_attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1606</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1606</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_NAME_1607</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILL_DESC_1607</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>heal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtarget,3000,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eventtarget,1006,particles/taken-gem.plist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemy,4001,particles/taken-gem.plist,1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enemy,1005,particles/taken-gem.plist,1,particles/taken-gem.plist</t>
+    <t>active</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3105,11 +3101,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3183,6 +3184,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3217,6 +3219,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3392,14 +3395,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="5" width="17.625" customWidth="1"/>
     <col min="6" max="6" width="13.875" bestFit="1" customWidth="1"/>
@@ -3412,7 +3415,7 @@
     <col min="16" max="16" width="130.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -3462,7 +3465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -3503,16 +3506,16 @@
         <v>19</v>
       </c>
       <c r="N2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O2" t="s">
         <v>18</v>
       </c>
       <c r="P2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -3520,22 +3523,22 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -3547,45 +3550,45 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" t="s">
         <v>60</v>
       </c>
-      <c r="M3" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" t="s">
-        <v>62</v>
-      </c>
       <c r="P3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1002</v>
       </c>
       <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
         <v>80</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I4">
         <v>10</v>
@@ -3597,45 +3600,45 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
         <v>86</v>
       </c>
-      <c r="N4" t="s">
-        <v>87</v>
-      </c>
-      <c r="O4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" t="s">
-        <v>88</v>
-      </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1200</v>
       </c>
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
         <v>50</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>51</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>52</v>
-      </c>
-      <c r="G5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" t="s">
-        <v>54</v>
       </c>
       <c r="I5">
         <v>10</v>
@@ -3647,22 +3650,22 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" t="s">
         <v>34</v>
       </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
       <c r="P5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1201</v>
       </c>
@@ -3670,22 +3673,22 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
         <v>90</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>91</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" t="s">
-        <v>93</v>
-      </c>
       <c r="H6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I6">
         <v>10</v>
@@ -3697,22 +3700,22 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" t="s">
         <v>94</v>
       </c>
-      <c r="O6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" t="s">
-        <v>96</v>
-      </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1202</v>
       </c>
@@ -3720,22 +3723,22 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I7">
         <v>10</v>
@@ -3747,22 +3750,22 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N7" t="s">
+        <v>92</v>
+      </c>
+      <c r="O7" t="s">
         <v>100</v>
       </c>
-      <c r="M7" t="s">
+      <c r="P7" t="s">
         <v>101</v>
       </c>
-      <c r="N7" t="s">
-        <v>94</v>
-      </c>
-      <c r="O7" t="s">
-        <v>102</v>
-      </c>
-      <c r="P7" t="s">
-        <v>103</v>
-      </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1203</v>
       </c>
@@ -3770,22 +3773,22 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I8">
         <v>10</v>
@@ -3797,45 +3800,45 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8" t="s">
         <v>92</v>
       </c>
-      <c r="M8" t="s">
-        <v>86</v>
-      </c>
-      <c r="N8" t="s">
-        <v>94</v>
-      </c>
       <c r="O8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1400</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
         <v>38</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>40</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>41</v>
       </c>
       <c r="I9">
         <v>10</v>
@@ -3847,22 +3850,22 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1401</v>
       </c>
@@ -3870,19 +3873,19 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
         <v>66</v>
       </c>
-      <c r="D10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>68</v>
-      </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
         <v>8</v>
@@ -3897,22 +3900,22 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M10" t="s">
         <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1600</v>
       </c>
@@ -3920,22 +3923,22 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
         <v>30</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11">
         <v>10</v>
@@ -3947,22 +3950,22 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" t="s">
         <v>33</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" t="s">
         <v>34</v>
       </c>
-      <c r="N11" t="s">
-        <v>78</v>
-      </c>
-      <c r="O11" t="s">
-        <v>35</v>
-      </c>
       <c r="P11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1601</v>
       </c>
@@ -3970,19 +3973,19 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
         <v>72</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>73</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>75</v>
       </c>
       <c r="H12" t="s">
         <v>8</v>
@@ -3997,22 +4000,22 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" t="s">
         <v>77</v>
       </c>
-      <c r="N12" t="s">
-        <v>79</v>
-      </c>
       <c r="O12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1602</v>
       </c>
@@ -4020,22 +4023,22 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
         <v>107</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>108</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>109</v>
-      </c>
-      <c r="G13" t="s">
-        <v>110</v>
-      </c>
-      <c r="H13" t="s">
-        <v>111</v>
       </c>
       <c r="I13">
         <v>10</v>
@@ -4047,22 +4050,22 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1603</v>
       </c>
@@ -4070,22 +4073,22 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I14">
         <v>10</v>
@@ -4097,22 +4100,22 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1605</v>
       </c>
@@ -4120,22 +4123,22 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I15">
         <v>10</v>
@@ -4147,22 +4150,22 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1606</v>
       </c>
@@ -4170,19 +4173,19 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
         <v>8</v>
@@ -4197,22 +4200,22 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" t="s">
         <v>34</v>
       </c>
-      <c r="N16" t="s">
-        <v>42</v>
-      </c>
-      <c r="O16" t="s">
-        <v>35</v>
-      </c>
       <c r="P16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>1607</v>
       </c>
@@ -4220,19 +4223,19 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" t="s">
         <v>8</v>
@@ -4247,22 +4250,22 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" t="s">
         <v>34</v>
       </c>
-      <c r="N17" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" t="s">
-        <v>35</v>
-      </c>
       <c r="P17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2000</v>
       </c>
@@ -4297,45 +4300,45 @@
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>28</v>
+        <v>182</v>
       </c>
       <c r="M18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="O18" t="s">
+        <v>124</v>
+      </c>
+      <c r="P18" t="s">
         <v>127</v>
       </c>
-      <c r="P18" t="s">
-        <v>130</v>
-      </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2400</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
         <v>43</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" t="s">
         <v>44</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" t="s">
-        <v>45</v>
       </c>
       <c r="I19">
         <v>10</v>
@@ -4347,45 +4350,45 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>46</v>
+        <v>183</v>
       </c>
       <c r="M19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3000</v>
       </c>
       <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
         <v>119</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
         <v>120</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" t="s">
         <v>121</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>122</v>
-      </c>
-      <c r="G20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" t="s">
-        <v>123</v>
       </c>
       <c r="I20">
         <v>10</v>
@@ -4397,22 +4400,22 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="M20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N20" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O20" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="P20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>3001</v>
       </c>
@@ -4420,10 +4423,10 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -4435,7 +4438,7 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I21">
         <v>10</v>
@@ -4447,22 +4450,22 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="M21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3002</v>
       </c>
@@ -4470,10 +4473,10 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -4482,7 +4485,7 @@
         <v>26</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H22" t="s">
         <v>8</v>
@@ -4497,22 +4500,22 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="M22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3003</v>
       </c>
@@ -4520,22 +4523,22 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23" t="s">
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I23">
         <v>10</v>
@@ -4547,22 +4550,22 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="M23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3004</v>
       </c>
@@ -4570,10 +4573,10 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4597,22 +4600,22 @@
         <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3005</v>
       </c>
@@ -4620,10 +4623,10 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -4632,7 +4635,7 @@
         <v>6</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25" t="s">
         <v>8</v>
@@ -4647,22 +4650,22 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P25" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3006</v>
       </c>
@@ -4670,22 +4673,22 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D26" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" t="s">
         <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I26">
         <v>10</v>
@@ -4697,22 +4700,22 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M26" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26" t="s">
+        <v>76</v>
+      </c>
+      <c r="O26" t="s">
         <v>34</v>
       </c>
-      <c r="N26" t="s">
-        <v>78</v>
-      </c>
-      <c r="O26" t="s">
-        <v>35</v>
-      </c>
       <c r="P26" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3007</v>
       </c>
@@ -4720,22 +4723,22 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D27" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G27" t="s">
         <v>16</v>
       </c>
       <c r="H27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I27">
         <v>10</v>
@@ -4747,22 +4750,22 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M27" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27" t="s">
+        <v>76</v>
+      </c>
+      <c r="O27" t="s">
         <v>34</v>
       </c>
-      <c r="N27" t="s">
-        <v>78</v>
-      </c>
-      <c r="O27" t="s">
-        <v>35</v>
-      </c>
       <c r="P27" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>4001</v>
       </c>
@@ -4770,16 +4773,16 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" t="s">
         <v>16</v>
@@ -4797,22 +4800,22 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>6000</v>
       </c>
@@ -4820,19 +4823,19 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H29" t="s">
         <v>8</v>
@@ -4847,22 +4850,22 @@
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="M29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>6001</v>
       </c>
@@ -4870,16 +4873,16 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G30" t="s">
         <v>16</v>
@@ -4897,22 +4900,22 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M30" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" t="s">
+        <v>41</v>
+      </c>
+      <c r="O30" t="s">
         <v>34</v>
       </c>
-      <c r="N30" t="s">
-        <v>42</v>
-      </c>
-      <c r="O30" t="s">
-        <v>35</v>
-      </c>
       <c r="P30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>6002</v>
       </c>
@@ -4920,16 +4923,16 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
         <v>16</v>
@@ -4947,22 +4950,22 @@
         <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M31" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" t="s">
+        <v>41</v>
+      </c>
+      <c r="O31" t="s">
         <v>34</v>
       </c>
-      <c r="N31" t="s">
-        <v>42</v>
-      </c>
-      <c r="O31" t="s">
-        <v>35</v>
-      </c>
       <c r="P31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>6003</v>
       </c>
@@ -4970,16 +4973,16 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
@@ -4997,22 +5000,22 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M32" t="s">
+        <v>33</v>
+      </c>
+      <c r="N32" t="s">
+        <v>41</v>
+      </c>
+      <c r="O32" t="s">
         <v>34</v>
       </c>
-      <c r="N32" t="s">
-        <v>42</v>
-      </c>
-      <c r="O32" t="s">
-        <v>35</v>
-      </c>
       <c r="P32" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>6004</v>
       </c>
@@ -5020,16 +5023,16 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G33" t="s">
         <v>16</v>
@@ -5047,19 +5050,19 @@
         <v>0</v>
       </c>
       <c r="L33" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="M33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N33" t="s">
+        <v>41</v>
+      </c>
+      <c r="O33" t="s">
         <v>34</v>
       </c>
-      <c r="N33" t="s">
-        <v>42</v>
-      </c>
-      <c r="O33" t="s">
-        <v>35</v>
-      </c>
       <c r="P33" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -5071,12 +5074,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5084,12 +5087,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>